<commit_message>
adding TITN risk factors to notes
</commit_message>
<xml_diff>
--- a/TITN/TITN.xlsx
+++ b/TITN/TITN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/32906c935fa0eb4f/models/TITN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1076" documentId="11_F25DC773A252ABDACC104889191A52245ADE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5FB40B10-298F-4E9C-B25E-49C2B5719DE6}"/>
+  <xr:revisionPtr revIDLastSave="1080" documentId="11_F25DC773A252ABDACC104889191A52245ADE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F37D250C-1888-4147-8CBE-42736F317F21}"/>
   <bookViews>
     <workbookView xWindow="19070" yWindow="5030" windowWidth="17190" windowHeight="15850" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,12 +37,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="119">
   <si>
     <t>Headquarters: West Fargo, ND</t>
-  </si>
-  <si>
-    <t># of Dealerships: 151 (2024)</t>
   </si>
   <si>
     <t>One of the largest dealers of agricultural and construction equipment, largest dealer for CNH in the world.</t>
@@ -444,7 +441,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -453,8 +450,6 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -739,27 +734,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:B4"/>
+  <dimension ref="B2:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -772,7 +762,7 @@
   <dimension ref="A1:Q125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -791,28 +781,28 @@
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L1" s="1">
         <v>2023</v>
@@ -822,25 +812,33 @@
       </c>
     </row>
     <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E3" s="9">
+        <v>118</v>
+      </c>
+      <c r="E3">
         <v>148</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="L3">
+        <f>E3</f>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="E4" s="8">
+        <v>117</v>
+      </c>
+      <c r="E4" s="4">
+        <v>3338</v>
+      </c>
+      <c r="L4" s="4">
+        <f>E4</f>
         <v>3338</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="2">
         <v>325660</v>
@@ -880,7 +878,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="2">
         <v>45458</v>
@@ -920,7 +918,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" s="2">
         <v>58258</v>
@@ -960,7 +958,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -994,7 +992,7 @@
     </row>
     <row r="10" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="3">
         <f>SUM(B6:B9)</f>
@@ -1047,7 +1045,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B11" s="2">
         <v>69547</v>
@@ -1087,7 +1085,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B12" s="2">
         <v>13664</v>
@@ -1127,7 +1125,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="2">
         <v>13395</v>
@@ -1167,7 +1165,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1201,7 +1199,7 @@
     </row>
     <row r="15" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15" s="3">
         <f>SUM(B11:B14)</f>
@@ -1251,7 +1249,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="2">
         <v>26266</v>
@@ -1291,7 +1289,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B17" s="2">
         <v>6336</v>
@@ -1331,7 +1329,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B18" s="2">
         <v>2331</v>
@@ -1371,7 +1369,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1405,7 +1403,7 @@
     </row>
     <row r="20" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B20" s="3">
         <f>SUM(B16:B19)</f>
@@ -1455,7 +1453,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B21" s="2">
         <v>1167</v>
@@ -1495,7 +1493,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B22" s="2">
         <v>360</v>
@@ -1535,7 +1533,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B23" s="2">
         <v>359</v>
@@ -1575,7 +1573,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1609,7 +1607,7 @@
     </row>
     <row r="25" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B25" s="3">
         <f>SUM(B21:B24)</f>
@@ -1659,7 +1657,7 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B26" s="2">
         <v>555</v>
@@ -1699,7 +1697,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B27" s="2">
         <v>6178</v>
@@ -1739,7 +1737,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B28" s="2">
         <v>97</v>
@@ -1779,7 +1777,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1806,7 +1804,7 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B30" s="3">
         <f>SUM(B26:B29)</f>
@@ -1856,7 +1854,7 @@
     </row>
     <row r="31" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B31" s="3">
         <f>B30+B25+B20+B15+B10</f>
@@ -1951,17 +1949,17 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B36" s="2">
         <v>429376</v>
@@ -2001,7 +1999,7 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B37" s="2">
         <v>96606</v>
@@ -2041,7 +2039,7 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B38" s="2">
         <v>34933</v>
@@ -2081,7 +2079,7 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B39" s="2">
         <v>8716</v>
@@ -2121,7 +2119,7 @@
     </row>
     <row r="40" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B40" s="3">
         <f>SUM(B36:B39)</f>
@@ -2171,7 +2169,7 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B41" s="2">
         <v>368262</v>
@@ -2210,7 +2208,7 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B42" s="2">
         <v>65103</v>
@@ -2249,7 +2247,7 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B43" s="2">
         <v>12409</v>
@@ -2288,7 +2286,7 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B44" s="2">
         <v>5277</v>
@@ -2327,7 +2325,7 @@
     </row>
     <row r="45" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B45" s="3">
         <f>SUM(B41:B44)</f>
@@ -2377,7 +2375,7 @@
     </row>
     <row r="46" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B46" s="3">
         <f>B36-B41</f>
@@ -2428,7 +2426,7 @@
     </row>
     <row r="47" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B47" s="3">
         <f t="shared" ref="B47:B49" si="24">B37-B42</f>
@@ -2479,7 +2477,7 @@
     </row>
     <row r="48" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B48" s="3">
         <f t="shared" si="24"/>
@@ -2530,7 +2528,7 @@
     </row>
     <row r="49" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B49" s="3">
         <f t="shared" si="24"/>
@@ -2581,7 +2579,7 @@
     </row>
     <row r="50" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B50" s="3">
         <f>SUM(B46:B49)</f>
@@ -2631,7 +2629,7 @@
     </row>
     <row r="51" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B51" s="2">
         <v>81315</v>
@@ -2669,7 +2667,7 @@
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -2693,7 +2691,7 @@
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E53" s="2"/>
       <c r="G53">
@@ -2714,7 +2712,7 @@
     </row>
     <row r="54" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B54" s="3">
         <f>B50-B51-B52-B53</f>
@@ -2765,7 +2763,7 @@
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B55" s="2">
         <v>720</v>
@@ -2809,7 +2807,7 @@
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B56" s="2">
         <v>-1272</v>
@@ -2853,7 +2851,7 @@
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B57" s="2">
         <v>-1274</v>
@@ -2897,7 +2895,7 @@
     </row>
     <row r="58" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B58" s="3">
         <f>B54+SUM(B55:B57)</f>
@@ -2947,7 +2945,7 @@
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B59" s="2">
         <v>8474</v>
@@ -2986,7 +2984,7 @@
     </row>
     <row r="60" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B60" s="3">
         <f>B58-B59</f>
@@ -3046,7 +3044,7 @@
     </row>
     <row r="62" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B62" s="5">
         <f>B60/B65</f>
@@ -3091,7 +3089,7 @@
     </row>
     <row r="63" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B63" s="5">
         <f>B60/B66</f>
@@ -3146,7 +3144,7 @@
     </row>
     <row r="65" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B65" s="4">
         <v>22441</v>
@@ -3175,7 +3173,7 @@
     </row>
     <row r="66" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B66" s="4">
         <v>22448</v>
@@ -3256,12 +3254,12 @@
     </row>
     <row r="69" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B70" s="2">
         <v>26965</v>
@@ -3304,7 +3302,7 @@
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B71" s="2">
         <v>6948</v>
@@ -3347,7 +3345,7 @@
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B72" s="2">
         <v>0</v>
@@ -3387,7 +3385,7 @@
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B73" s="2">
         <v>-904</v>
@@ -3430,7 +3428,7 @@
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B74" s="2">
         <v>659</v>
@@ -3473,7 +3471,7 @@
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B75" s="2">
         <v>64</v>
@@ -3516,7 +3514,7 @@
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -3537,7 +3535,7 @@
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -3570,7 +3568,7 @@
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B78" s="2">
         <v>0</v>
@@ -3610,7 +3608,7 @@
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B79" s="2">
         <v>0</v>
@@ -3650,7 +3648,7 @@
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B80" s="2">
         <v>1663</v>
@@ -3694,7 +3692,7 @@
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B81" s="2">
         <v>-32307</v>
@@ -3737,7 +3735,7 @@
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B82" s="2">
         <v>1274</v>
@@ -3780,7 +3778,7 @@
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B83" s="2">
         <v>-140107</v>
@@ -3823,7 +3821,7 @@
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B84" s="2">
         <v>86259</v>
@@ -3866,7 +3864,7 @@
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B85" s="2">
         <v>-23987</v>
@@ -3909,7 +3907,7 @@
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B86" s="2">
         <v>-4231</v>
@@ -3952,7 +3950,7 @@
     </row>
     <row r="87" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B87" s="3">
         <f>SUM(B70:B86)</f>
@@ -4054,7 +4052,7 @@
     </row>
     <row r="90" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
@@ -4067,7 +4065,7 @@
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B91" s="2">
         <v>38357</v>
@@ -4103,7 +4101,7 @@
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B92" s="2">
         <v>131284</v>
@@ -4139,7 +4137,7 @@
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B93" s="2">
         <v>854154</v>
@@ -4175,7 +4173,7 @@
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B94" s="2">
         <v>19792</v>
@@ -4211,7 +4209,7 @@
     </row>
     <row r="95" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B95" s="3">
         <f>SUM(B91:B94)</f>
@@ -4257,7 +4255,7 @@
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B96" s="2">
         <v>233830</v>
@@ -4293,7 +4291,7 @@
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B97" s="2">
         <v>47684</v>
@@ -4329,7 +4327,7 @@
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B98" s="2">
         <v>2169</v>
@@ -4365,7 +4363,7 @@
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B99" s="2">
         <v>30691</v>
@@ -4401,7 +4399,7 @@
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B100" s="2">
         <v>18330</v>
@@ -4437,7 +4435,7 @@
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B101" s="2">
         <v>1814</v>
@@ -4473,7 +4471,7 @@
     </row>
     <row r="102" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B102" s="3">
         <f>SUM(B96:B101)</f>
@@ -4519,7 +4517,7 @@
     </row>
     <row r="103" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B103" s="3">
         <f>B95+B102</f>
@@ -4565,7 +4563,7 @@
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B104" s="2">
         <v>43195</v>
@@ -4601,7 +4599,7 @@
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B105" s="2">
         <v>442950</v>
@@ -4637,7 +4635,7 @@
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B106" s="2">
         <v>7481</v>
@@ -4673,7 +4671,7 @@
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B107" s="2">
         <v>9888</v>
@@ -4709,7 +4707,7 @@
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B108" s="2">
         <v>97532</v>
@@ -4745,7 +4743,7 @@
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B109" s="2">
         <v>48042</v>
@@ -4781,7 +4779,7 @@
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B110" s="2">
         <v>11151</v>
@@ -4806,7 +4804,7 @@
     </row>
     <row r="111" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B111" s="3">
         <f t="shared" ref="B111:I111" si="63">SUM(B104:B110)</f>
@@ -4852,7 +4850,7 @@
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B112" s="2">
         <v>93445</v>
@@ -4888,7 +4886,7 @@
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B113" s="2">
         <v>45770</v>
@@ -4924,7 +4922,7 @@
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B114" s="2">
         <v>9567</v>
@@ -4960,7 +4958,7 @@
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B115" s="2">
         <v>5051</v>
@@ -4996,7 +4994,7 @@
     </row>
     <row r="116" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B116" s="3">
         <f>SUM(B112:B115)</f>
@@ -5042,7 +5040,7 @@
     </row>
     <row r="117" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B117" s="3">
         <f>B116+B111</f>
@@ -5088,7 +5086,7 @@
     </row>
     <row r="118" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B118" s="2">
         <v>256207</v>
@@ -5124,7 +5122,7 @@
     </row>
     <row r="119" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B119" s="2">
         <v>311749</v>
@@ -5160,7 +5158,7 @@
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B120" s="2">
         <v>-3923</v>
@@ -5196,7 +5194,7 @@
     </row>
     <row r="121" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A121" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B121" s="3">
         <f>SUM(B118:B120)</f>
@@ -5242,7 +5240,7 @@
     </row>
     <row r="122" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B122" s="3">
         <f>B121+B117</f>
@@ -5288,7 +5286,7 @@
     </row>
     <row r="124" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B124" s="3">
         <f>B93-B105</f>
@@ -5334,7 +5332,7 @@
     </row>
     <row r="125" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B125" s="6">
         <f>B93/B105</f>

</xml_diff>

<commit_message>
added TITN Notes, Risks, model info
</commit_message>
<xml_diff>
--- a/TITN/TITN.xlsx
+++ b/TITN/TITN.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/32906c935fa0eb4f/models/TITN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1080" documentId="11_F25DC773A252ABDACC104889191A52245ADE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F37D250C-1888-4147-8CBE-42736F317F21}"/>
+  <xr:revisionPtr revIDLastSave="1106" documentId="11_F25DC773A252ABDACC104889191A52245ADE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46B564C4-FCFD-4566-9979-0C521EFB9AE0}"/>
   <bookViews>
-    <workbookView xWindow="19070" yWindow="5030" windowWidth="17190" windowHeight="15850" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20770" yWindow="4940" windowWidth="17190" windowHeight="15850" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
-    <sheet name="model" sheetId="2" r:id="rId2"/>
+    <sheet name="todo" sheetId="4" r:id="rId2"/>
+    <sheet name="M&amp;A" sheetId="5" r:id="rId3"/>
+    <sheet name="model" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="124">
   <si>
     <t>Headquarters: West Fargo, ND</t>
   </si>
@@ -394,6 +396,21 @@
   </si>
   <si>
     <t>Locations</t>
+  </si>
+  <si>
+    <t>Python script to show some graphs - histograms, delta of revenues, CFFO, other useful ratios.</t>
+  </si>
+  <si>
+    <t>Web framework to view everything: Notes, models, etc. - 'real time' stock price and/or news feed on stock ticker/business.</t>
+  </si>
+  <si>
+    <t>Purchased J.J. O'Connor &amp; Sons Pty. Ltd. 15 CaseIH dealerships located in Australia. $66.5M cash paid - financed through available cash resources and LOC.</t>
+  </si>
+  <si>
+    <t>*Purchase of JJ O'Connor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purchaed Heartland Agriculture, LLC, Heartland Solutions, LLC, and Heartland Leveraged Lender, LLC. 12 CaseIH commercial application ag locations. Opportunities for synergies due to overlap of footprints to package deals that include both commercial application equipment and other ag equipment to commercial customers. Purchased for $94.4M, financed through cash resources and LOC availability. </t>
   </si>
 </sst>
 </file>
@@ -441,7 +458,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -450,6 +467,9 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -758,11 +778,77 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A532B8A9-72BD-4CFE-8449-3B24FC76CA39}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.7265625" style="8"/>
+    <col min="2" max="2" width="104.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="8">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="8">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01EA54E0-299A-42E8-83C7-403ECF34C403}">
+  <dimension ref="B2:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49AC6758-3054-45BD-A746-0979BE500444}">
   <dimension ref="A1:Q125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -836,6 +922,11 @@
         <v>3338</v>
       </c>
     </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E5" t="s">
+        <v>122</v>
+      </c>
+    </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>26</v>

</xml_diff>